<commit_message>
Update Rezultate Biostat 2
</commit_message>
<xml_diff>
--- a/Teaching/Biostatistics/results/Tabel_Biostatistica - Prezenta Examen.xlsx
+++ b/Teaching/Biostatistics/results/Tabel_Biostatistica - Prezenta Examen.xlsx
@@ -1735,7 +1735,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1959,12 +1959,15 @@
       <c r="C9">
         <v>503</v>
       </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
       <c r="E9">
         <v>1.5</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -2028,14 +2031,14 @@
         <v>503</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12">
         <v>1.5</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -2189,12 +2192,15 @@
       <c r="C18">
         <v>503</v>
       </c>
+      <c r="D18">
+        <v>2.25</v>
+      </c>
       <c r="E18">
         <v>1.5</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G18">
         <v>1</v>

</xml_diff>